<commit_message>
Completed implementation of RQ3 for both regular and micro-clones.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1FCF3B-035F-46AF-A0F2-D4A512A84799}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C15066-2CC5-4D88-B7AB-6BA99003E65D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14175" yWindow="7440" windowWidth="12975" windowHeight="6015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12810" yWindow="4890" windowWidth="12975" windowHeight="6015" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA0352E-0786-42C8-B957-A5D601AF8293}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,13 +1113,25 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>86</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>96.511627906976756</v>
+      </c>
+      <c r="E3">
+        <v>1225</v>
+      </c>
+      <c r="F3">
+        <v>13401</v>
+      </c>
+      <c r="G3">
         <f>E3/F3*100</f>
-        <v>#DIV/0!</v>
+        <v>9.1411088724722038</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,27 +1217,27 @@
       </c>
       <c r="B9">
         <f>SUM(B3:B8)</f>
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="C9">
         <f>SUM(C3:C8)</f>
-        <v>67</v>
+        <v>153</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>94.029850746268664</v>
+        <v>95.424836601307192</v>
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>525</v>
+        <v>1750</v>
       </c>
       <c r="F9">
         <f>SUM(F3:F8)</f>
-        <v>4335</v>
+        <v>17736</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>12.110726643598616</v>
+        <v>9.8669373026612543</v>
       </c>
     </row>
   </sheetData>
@@ -1242,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F3B9B-1193-44AD-896D-0D732F97E1BA}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,13 +1317,25 @@
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4:D9" si="0">B4/C4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>72</v>
+      </c>
+      <c r="F4">
+        <v>72</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4:G9" si="1">E4/F4*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,27 +1396,27 @@
       </c>
       <c r="B9">
         <f>SUM(B3:B8)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <f>SUM(C3:C8)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" t="e">
+        <v>12</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="F9">
         <f>SUM(F3:F8)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>72</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation of RQ4 for both regular and micro-clones are completed.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C15066-2CC5-4D88-B7AB-6BA99003E65D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB456EE-CE45-46D4-828A-E3C526BB25CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12810" yWindow="4890" windowWidth="12975" windowHeight="6015" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13305" yWindow="7470" windowWidth="14925" windowHeight="6015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F3B9B-1193-44AD-896D-0D732F97E1BA}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,13 +1304,25 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>129</v>
+      </c>
+      <c r="F3">
+        <v>129</v>
+      </c>
+      <c r="G3">
         <f>E3/F3*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1396,11 +1408,11 @@
       </c>
       <c r="B9">
         <f>SUM(B3:B8)</f>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <f>SUM(C3:C8)</f>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -1408,11 +1420,11 @@
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>72</v>
+        <v>201</v>
       </c>
       <c r="F9">
         <f>SUM(F3:F8)</f>
-        <v>72</v>
+        <v>201</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
@@ -1433,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45DAA6C-6044-4BDB-98CB-11DB5B63E69A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,26 +1496,44 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="D3">
         <f>C3/B3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>129</v>
+      </c>
+      <c r="G3">
         <f>F3/E3*100</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4:D7" si="0">C4/B4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="E4">
+        <v>72</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4:G9" si="1">F4/E4*100</f>
-        <v>#DIV/0!</v>
+        <v>13.888888888888889</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1564,27 +1594,27 @@
       </c>
       <c r="B9">
         <f>SUM(B3:B8)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C9">
         <f>SUM(C3:C8)</f>
-        <v>0</v>
-      </c>
-      <c r="D9" t="e">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <f>C9/B9*100</f>
-        <v>#DIV/0!</v>
+        <v>7.1428571428571423</v>
       </c>
       <c r="E9">
         <f>SUM(E3:E8)</f>
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="F9">
         <f>SUM(F3:F8)</f>
-        <v>0</v>
-      </c>
-      <c r="G9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>4.9751243781094532</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Result updated for Jabref, RQ1.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB6CBB9-809F-43DB-BDD6-F196BF3C7880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAD98B-2EB4-4A40-B7BE-3A176E3E8122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13305" yWindow="7470" windowWidth="14925" windowHeight="6015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12675" yWindow="4290" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>Ctags</t>
   </si>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +913,7 @@
         <v>73</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E9" si="0">C4/D4</f>
+        <f t="shared" ref="E4" si="0">C4/D4</f>
         <v>0.53424657534246578</v>
       </c>
       <c r="F4">
@@ -923,101 +923,97 @@
         <v>73</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H9" si="1">F4/G4</f>
+        <f t="shared" ref="H4" si="1">F4/G4</f>
         <v>7.2191780821917808</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1110</v>
+        <v>10354</v>
       </c>
       <c r="E5" t="e">
-        <f t="shared" si="0"/>
+        <f>C5/D5</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H5" t="e">
-        <f t="shared" si="1"/>
+        <f>F5/G5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>10354</v>
+        <v>2886</v>
       </c>
       <c r="E6" t="e">
-        <f t="shared" si="0"/>
+        <f>C6/D6</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H6" t="e">
-        <f t="shared" si="1"/>
+        <f>F6/G6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>2886</v>
-      </c>
-      <c r="E7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2798</v>
+      </c>
+      <c r="C7">
+        <v>165</v>
+      </c>
+      <c r="D7">
+        <v>148</v>
+      </c>
+      <c r="E7">
+        <f>C7/D7</f>
+        <v>1.1148648648648649</v>
+      </c>
+      <c r="F7">
+        <v>1804</v>
+      </c>
+      <c r="G7">
+        <v>148</v>
+      </c>
+      <c r="H7">
+        <f>F7/G7</f>
+        <v>12.189189189189189</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>2798</v>
-      </c>
-      <c r="E8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
-        <f>SUM(C3:C8)</f>
-        <v>122</v>
-      </c>
-      <c r="D9">
-        <f>SUM(D3:D8)</f>
-        <v>205</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0.59512195121951217</v>
-      </c>
-      <c r="F9">
-        <f>SUM(F3:F8)</f>
-        <v>1752</v>
-      </c>
-      <c r="G9">
-        <f>SUM(G3:G8)</f>
-        <v>205</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>8.5463414634146346</v>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>287</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D3:D7)</f>
+        <v>353</v>
+      </c>
+      <c r="E8">
+        <f>C8/D8</f>
+        <v>0.81303116147308785</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>3556</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G3:G7)</f>
+        <v>353</v>
+      </c>
+      <c r="H8">
+        <f>F8/G8</f>
+        <v>10.073654390934845</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1445,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45DAA6C-6044-4BDB-98CB-11DB5B63E69A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Included getClassIDMicro() and isClonePairBinaryMicro().
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAD98B-2EB4-4A40-B7BE-3A176E3E8122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA503B0C-5D35-484F-B25B-5C2658BD88A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="4290" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12555" yWindow="5460" windowWidth="14925" windowHeight="6015" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
     <sheet name="RQ2" sheetId="2" r:id="rId2"/>
     <sheet name="RQ3" sheetId="3" r:id="rId3"/>
     <sheet name="RQ4" sheetId="4" r:id="rId4"/>
+    <sheet name="RQ1a" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,15 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
   <si>
     <t>Ctags</t>
   </si>
   <si>
     <t>Brlcad</t>
-  </si>
-  <si>
-    <t>MonoOSC</t>
   </si>
   <si>
     <t>Freecol</t>
@@ -810,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,12 +830,12 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -850,25 +848,25 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -929,7 +927,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>10354</v>
@@ -945,7 +943,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2886</v>
@@ -961,7 +959,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2798</v>
@@ -989,7 +987,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
@@ -1058,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA0352E-0786-42C8-B957-A5D601AF8293}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,12 +1072,12 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1087,22 +1085,22 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,7 +1139,7 @@
         <v>67</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">B4/C4*100</f>
+        <f t="shared" ref="D4" si="0">B4/C4*100</f>
         <v>94.029850746268664</v>
       </c>
       <c r="E4">
@@ -1151,7 +1149,7 @@
         <v>4335</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="1">E4/F4*100</f>
+        <f t="shared" ref="G4" si="1">E4/F4*100</f>
         <v>12.110726643598616</v>
       </c>
     </row>
@@ -1160,11 +1158,11 @@
         <v>2</v>
       </c>
       <c r="D5" t="e">
-        <f t="shared" si="0"/>
+        <f>B5/C5*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G5" t="e">
-        <f t="shared" si="1"/>
+        <f>E5/F5*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1173,11 +1171,11 @@
         <v>3</v>
       </c>
       <c r="D6" t="e">
-        <f t="shared" si="0"/>
+        <f>B6/C6*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G6" t="e">
-        <f t="shared" si="1"/>
+        <f>E6/F6*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1186,53 +1184,40 @@
         <v>4</v>
       </c>
       <c r="D7" t="e">
-        <f t="shared" si="0"/>
+        <f>B7/C7*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G7" t="e">
-        <f t="shared" si="1"/>
+        <f>E7/F7*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <f>SUM(B3:B8)</f>
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
         <v>146</v>
       </c>
-      <c r="C9">
-        <f>SUM(C3:C8)</f>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
         <v>153</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
+      <c r="D8">
+        <f>B8/C8*100</f>
         <v>95.424836601307192</v>
       </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
         <v>1750</v>
       </c>
-      <c r="F9">
-        <f>SUM(F3:F8)</f>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
         <v>17736</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
+      <c r="G8">
+        <f>E8/F8*100</f>
         <v>9.8669373026612543</v>
       </c>
     </row>
@@ -1248,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16F3B9B-1193-44AD-896D-0D732F97E1BA}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,12 +1250,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1278,22 +1263,22 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,7 +1317,7 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" si="0">B4/C4*100</f>
+        <f t="shared" ref="D4" si="0">B4/C4*100</f>
         <v>100</v>
       </c>
       <c r="E4">
@@ -1342,7 +1327,7 @@
         <v>72</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="1">E4/F4*100</f>
+        <f t="shared" ref="G4" si="1">E4/F4*100</f>
         <v>100</v>
       </c>
     </row>
@@ -1351,11 +1336,11 @@
         <v>2</v>
       </c>
       <c r="D5" t="e">
-        <f t="shared" si="0"/>
+        <f>B5/C5*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G5" t="e">
-        <f t="shared" si="1"/>
+        <f>E5/F5*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1364,11 +1349,11 @@
         <v>3</v>
       </c>
       <c r="D6" t="e">
-        <f t="shared" si="0"/>
+        <f>B6/C6*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G6" t="e">
-        <f t="shared" si="1"/>
+        <f>E6/F6*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1377,53 +1362,40 @@
         <v>4</v>
       </c>
       <c r="D7" t="e">
-        <f t="shared" si="0"/>
+        <f>B7/C7*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G7" t="e">
-        <f t="shared" si="1"/>
+        <f>E7/F7*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <f>SUM(B3:B8)</f>
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
         <v>28</v>
       </c>
-      <c r="C9">
-        <f>SUM(C3:C8)</f>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
         <v>28</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
+      <c r="D8">
+        <f>B8/C8*100</f>
         <v>100</v>
       </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
         <v>201</v>
       </c>
-      <c r="F9">
-        <f>SUM(F3:F8)</f>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
         <v>201</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
+      <c r="G8">
+        <f>E8/F8*100</f>
         <v>100</v>
       </c>
     </row>
@@ -1442,7 +1414,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,34 +1430,34 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1524,7 +1496,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D7" si="0">C4/B4*100</f>
+        <f t="shared" ref="D4" si="0">C4/B4*100</f>
         <v>16.666666666666664</v>
       </c>
       <c r="E4">
@@ -1534,7 +1506,7 @@
         <v>10</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G9" si="1">F4/E4*100</f>
+        <f t="shared" ref="G4" si="1">F4/E4*100</f>
         <v>13.888888888888889</v>
       </c>
     </row>
@@ -1543,11 +1515,11 @@
         <v>2</v>
       </c>
       <c r="D5" t="e">
-        <f t="shared" si="0"/>
+        <f>C5/B5*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G5" t="e">
-        <f t="shared" si="1"/>
+        <f>F5/E5*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1560,7 +1532,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G6" t="e">
-        <f t="shared" si="1"/>
+        <f>F6/E6*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1569,7 +1541,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="e">
-        <f t="shared" si="0"/>
+        <f>C7/B7*100</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G7" t="e">
@@ -1579,53 +1551,40 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="e">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>9</v>
+      </c>
+      <c r="D8">
         <f>C8/B8*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <f>SUM(B3:B8)</f>
-        <v>28</v>
-      </c>
-      <c r="C9">
-        <f>SUM(C3:C8)</f>
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <f>C9/B9*100</f>
         <v>32.142857142857146</v>
       </c>
-      <c r="E9">
-        <f>SUM(E3:E8)</f>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
         <v>201</v>
       </c>
-      <c r="F9">
-        <f>SUM(F3:F8)</f>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
         <v>48</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
+      <c r="G8">
+        <f>F8/E8*100</f>
         <v>23.880597014925371</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="e">
-        <f>AVERAGE(D3:D8)</f>
+        <f>AVERAGE(D3:D7)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G15" t="e">
-        <f>AVERAGE(G3:G8)</f>
+        <f>AVERAGE(G3:G7)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1637,4 +1596,183 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F880183A-EC63-487C-ABC7-6BFBFB289FA5}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1126</v>
+      </c>
+      <c r="E3" t="e">
+        <f>C3/D3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" t="e">
+        <f>F3/G3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1041</v>
+      </c>
+      <c r="C4">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4" si="0">C4/D4</f>
+        <v>2.4230769230769229</v>
+      </c>
+      <c r="F4">
+        <v>113</v>
+      </c>
+      <c r="G4">
+        <v>26</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4" si="1">F4/G4</f>
+        <v>4.3461538461538458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>10354</v>
+      </c>
+      <c r="E5" t="e">
+        <f>C5/D5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" t="e">
+        <f>F5/G5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2886</v>
+      </c>
+      <c r="E6" t="e">
+        <f>C6/D6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" t="e">
+        <f>F6/G6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>2798</v>
+      </c>
+      <c r="E7" t="e">
+        <f>C7/D7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="e">
+        <f>F7/G7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D3:D7)</f>
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <f>C8/D8</f>
+        <v>2.4230769230769229</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>113</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G3:G7)</f>
+        <v>26</v>
+      </c>
+      <c r="H8">
+        <f>F8/G8</f>
+        <v>4.3461538461538458</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated result of RQ1 for Ctags.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA503B0C-5D35-484F-B25B-5C2658BD88A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F56E35-966A-44BE-B137-99A237B4B0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12555" yWindow="5460" windowWidth="14925" windowHeight="6015" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="480" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
     <sheet name="RQ2" sheetId="2" r:id="rId2"/>
     <sheet name="RQ3" sheetId="3" r:id="rId3"/>
     <sheet name="RQ4" sheetId="4" r:id="rId4"/>
-    <sheet name="RQ1a" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>Ctags</t>
   </si>
@@ -808,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,21 +879,21 @@
         <v>83</v>
       </c>
       <c r="D3">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="E3">
         <f>C3/D3</f>
-        <v>0.62878787878787878</v>
+        <v>2.1282051282051282</v>
       </c>
       <c r="F3">
-        <v>1225</v>
+        <v>208</v>
       </c>
       <c r="G3">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="H3">
         <f>F3/G3</f>
-        <v>9.2803030303030312</v>
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -905,24 +904,24 @@
         <v>1041</v>
       </c>
       <c r="C4">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="D4">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4" si="0">C4/D4</f>
-        <v>0.53424657534246578</v>
+        <v>2.4230769230769229</v>
       </c>
       <c r="F4">
-        <v>527</v>
+        <v>113</v>
       </c>
       <c r="G4">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4" si="1">F4/G4</f>
-        <v>7.2191780821917808</v>
+        <v>4.3461538461538458</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -964,25 +963,13 @@
       <c r="B7">
         <v>2798</v>
       </c>
-      <c r="C7">
-        <v>165</v>
-      </c>
-      <c r="D7">
-        <v>148</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="e">
         <f>C7/D7</f>
-        <v>1.1148648648648649</v>
-      </c>
-      <c r="F7">
-        <v>1804</v>
-      </c>
-      <c r="G7">
-        <v>148</v>
-      </c>
-      <c r="H7">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" t="e">
         <f>F7/G7</f>
-        <v>12.189189189189189</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -991,27 +978,27 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>287</v>
+        <v>146</v>
       </c>
       <c r="D8">
         <f>SUM(D3:D7)</f>
-        <v>353</v>
+        <v>65</v>
       </c>
       <c r="E8">
         <f>C8/D8</f>
-        <v>0.81303116147308785</v>
+        <v>2.2461538461538462</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>3556</v>
+        <v>321</v>
       </c>
       <c r="G8">
         <f>SUM(G3:G7)</f>
-        <v>353</v>
+        <v>65</v>
       </c>
       <c r="H8">
         <f>F8/G8</f>
-        <v>10.073654390934845</v>
+        <v>4.9384615384615387</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1059,7 +1046,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,50 +1094,26 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>83</v>
-      </c>
-      <c r="C3">
-        <v>86</v>
-      </c>
-      <c r="D3">
+      <c r="D3" t="e">
         <f>B3/C3*100</f>
-        <v>96.511627906976756</v>
-      </c>
-      <c r="E3">
-        <v>1225</v>
-      </c>
-      <c r="F3">
-        <v>13401</v>
-      </c>
-      <c r="G3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
         <f>E3/F3*100</f>
-        <v>9.1411088724722038</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>63</v>
-      </c>
-      <c r="C4">
-        <v>67</v>
-      </c>
-      <c r="D4">
+      <c r="D4" t="e">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>94.029850746268664</v>
-      </c>
-      <c r="E4">
-        <v>525</v>
-      </c>
-      <c r="F4">
-        <v>4335</v>
-      </c>
-      <c r="G4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
-        <v>12.110726643598616</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1198,27 +1161,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>146</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>153</v>
-      </c>
-      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="e">
         <f>B8/C8*100</f>
-        <v>95.424836601307192</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>1750</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>17736</v>
-      </c>
-      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
         <f>E8/F8*100</f>
-        <v>9.8669373026612543</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1199,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,50 +1248,26 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>16</v>
-      </c>
-      <c r="D3">
+      <c r="D3" t="e">
         <f>B3/C3*100</f>
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>129</v>
-      </c>
-      <c r="F3">
-        <v>129</v>
-      </c>
-      <c r="G3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
         <f>E3/F3*100</f>
-        <v>100</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
+      <c r="D4" t="e">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>72</v>
-      </c>
-      <c r="F4">
-        <v>72</v>
-      </c>
-      <c r="G4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
-        <v>100</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1376,27 +1315,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>28</v>
-      </c>
-      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="e">
         <f>B8/C8*100</f>
-        <v>100</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>201</v>
-      </c>
-      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
         <f>E8/F8*100</f>
-        <v>100</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1353,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,50 +1403,26 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
+      <c r="D3" t="e">
         <f>C3/B3*100</f>
-        <v>43.75</v>
-      </c>
-      <c r="E3">
-        <v>129</v>
-      </c>
-      <c r="F3">
-        <v>38</v>
-      </c>
-      <c r="G3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" t="e">
         <f>F3/E3*100</f>
-        <v>29.457364341085274</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
+      <c r="D4" t="e">
         <f t="shared" ref="D4" si="0">C4/B4*100</f>
-        <v>16.666666666666664</v>
-      </c>
-      <c r="E4">
-        <v>72</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
         <f t="shared" ref="G4" si="1">F4/E4*100</f>
-        <v>13.888888888888889</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1555,27 +1470,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>9</v>
-      </c>
-      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="e">
         <f>C8/B8*100</f>
-        <v>32.142857142857146</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>48</v>
-      </c>
-      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="e">
         <f>F8/E8*100</f>
-        <v>23.880597014925371</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,183 +1511,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F880183A-EC63-487C-ABC7-6BFBFB289FA5}">
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1126</v>
-      </c>
-      <c r="E3" t="e">
-        <f>C3/D3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H3" t="e">
-        <f>F3/G3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1041</v>
-      </c>
-      <c r="C4">
-        <v>63</v>
-      </c>
-      <c r="D4">
-        <v>26</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="0">C4/D4</f>
-        <v>2.4230769230769229</v>
-      </c>
-      <c r="F4">
-        <v>113</v>
-      </c>
-      <c r="G4">
-        <v>26</v>
-      </c>
-      <c r="H4">
-        <f t="shared" ref="H4" si="1">F4/G4</f>
-        <v>4.3461538461538458</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>10354</v>
-      </c>
-      <c r="E5" t="e">
-        <f>C5/D5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" t="e">
-        <f>F5/G5</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>2886</v>
-      </c>
-      <c r="E6" t="e">
-        <f>C6/D6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" t="e">
-        <f>F6/G6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>2798</v>
-      </c>
-      <c r="E7" t="e">
-        <f>C7/D7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" t="e">
-        <f>F7/G7</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <f>SUM(C3:C7)</f>
-        <v>63</v>
-      </c>
-      <c r="D8">
-        <f>SUM(D3:D7)</f>
-        <v>26</v>
-      </c>
-      <c r="E8">
-        <f>C8/D8</f>
-        <v>2.4230769230769229</v>
-      </c>
-      <c r="F8">
-        <f>SUM(F3:F7)</f>
-        <v>113</v>
-      </c>
-      <c r="G8">
-        <f>SUM(G3:G7)</f>
-        <v>26</v>
-      </c>
-      <c r="H8">
-        <f>F8/G8</f>
-        <v>4.3461538461538458</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the system termination option to all methods.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F56E35-966A-44BE-B137-99A237B4B0DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F440FD3-5DAB-484A-806E-196622E8523B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="480" windowWidth="14925" windowHeight="6015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="480" windowWidth="14925" windowHeight="6015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -807,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,26 +1094,50 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>83</v>
+      </c>
+      <c r="C3">
+        <v>86</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>96.511627906976756</v>
+      </c>
+      <c r="E3">
+        <v>208</v>
+      </c>
+      <c r="F3">
+        <v>10411</v>
+      </c>
+      <c r="G3">
         <f>E3/F3*100</f>
-        <v>#DIV/0!</v>
+        <v>1.9978868504466432</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>63</v>
+      </c>
+      <c r="C4">
+        <v>67</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>94.029850746268664</v>
+      </c>
+      <c r="E4">
+        <v>113</v>
+      </c>
+      <c r="F4">
+        <v>2901</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
-        <v>#DIV/0!</v>
+        <v>3.8952085487762842</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1161,27 +1185,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>153</v>
+      </c>
+      <c r="D8">
         <f>B8/C8*100</f>
-        <v>#DIV/0!</v>
+        <v>95.424836601307192</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>321</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>13312</v>
+      </c>
+      <c r="G8">
         <f>E8/F8*100</f>
-        <v>#DIV/0!</v>
+        <v>2.4113581730769234</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +1223,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,26 +1272,50 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
         <f>B3/C3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>42</v>
+      </c>
+      <c r="G3">
         <f>E3/F3*100</f>
-        <v>#DIV/0!</v>
+        <v>78.571428571428569</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">B4/C4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4" si="1">E4/F4*100</f>
-        <v>#DIV/0!</v>
+        <v>78.571428571428569</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1315,27 +1363,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>28</v>
+      </c>
+      <c r="D8">
         <f>B8/C8*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>70</v>
+      </c>
+      <c r="G8">
         <f>E8/F8*100</f>
-        <v>#DIV/0!</v>
+        <v>78.571428571428569</v>
       </c>
     </row>
   </sheetData>
@@ -1352,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45DAA6C-6044-4BDB-98CB-11DB5B63E69A}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,26 +1451,50 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="e">
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
         <f>C3/B3*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" t="e">
+        <v>43.75</v>
+      </c>
+      <c r="E3">
+        <v>33</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
         <f>F3/E3*100</f>
-        <v>#DIV/0!</v>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="e">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <f t="shared" ref="D4" si="0">C4/B4*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" t="e">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
         <f t="shared" ref="G4" si="1">F4/E4*100</f>
-        <v>#DIV/0!</v>
+        <v>13.636363636363635</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1470,27 +1542,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>0</v>
-      </c>
-      <c r="D8" t="e">
+        <v>9</v>
+      </c>
+      <c r="D8">
         <f>C8/B8*100</f>
-        <v>#DIV/0!</v>
+        <v>32.142857142857146</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="G8" t="e">
+        <v>14</v>
+      </c>
+      <c r="G8">
         <f>F8/E8*100</f>
-        <v>#DIV/0!</v>
+        <v>25.454545454545453</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented RQ5 for both regular and micro clones.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F440FD3-5DAB-484A-806E-196622E8523B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7EAF14-62CA-4AE4-A815-72C2946F48E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="480" windowWidth="14925" windowHeight="6015" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14415" yWindow="3225" windowWidth="12525" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
@@ -146,400 +146,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>675385</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2315465" cy="628650"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A1B7C9-9C63-492E-A370-27B519FA45EC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8514460" y="2733676"/>
-              <a:ext cx="2315465" cy="628650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSup>
-                      <m:sSupPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-CA" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSupPr>
-                      <m:e>
-                        <m:d>
-                          <m:dPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-CA" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:dPr>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝐴𝑣𝑒𝑟𝑎𝑔𝑒</m:t>
-                            </m:r>
-                          </m:e>
-                        </m:d>
-                      </m:e>
-                      <m:sup/>
-                    </m:sSup>
-                    <m:r>
-                      <a:rPr lang="en-CA" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:f>
-                      <m:fPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:fPr>
-                      <m:num>
-                        <m:nary>
-                          <m:naryPr>
-                            <m:chr m:val="∑"/>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-CA" sz="1100" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:naryPr>
-                          <m:sub>
-                            <m:r>
-                              <m:rPr>
-                                <m:brk m:alnAt="23"/>
-                              </m:rPr>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑛</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>=</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>1</m:t>
-                            </m:r>
-                          </m:sub>
-                          <m:sup>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝑛</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>=6</m:t>
-                            </m:r>
-                          </m:sup>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:solidFill>
-                                  <a:schemeClr val="tx1"/>
-                                </a:solidFill>
-                                <a:effectLst/>
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                <a:ea typeface="+mn-ea"/>
-                                <a:cs typeface="+mn-cs"/>
-                              </a:rPr>
-                              <m:t>𝐶𝐹𝑛</m:t>
-                            </m:r>
-                          </m:e>
-                        </m:nary>
-                        <m:r>
-                          <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1"/>
-                            </a:solidFill>
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="+mn-ea"/>
-                            <a:cs typeface="+mn-cs"/>
-                          </a:rPr>
-                          <m:t>  </m:t>
-                        </m:r>
-                      </m:num>
-                      <m:den>
-                        <m:nary>
-                          <m:naryPr>
-                            <m:chr m:val="∑"/>
-                            <m:ctrlPr>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:naryPr>
-                          <m:sub>
-                            <m:r>
-                              <m:rPr>
-                                <m:brk m:alnAt="23"/>
-                              </m:rPr>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑛</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>=1</m:t>
-                            </m:r>
-                          </m:sub>
-                          <m:sup>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑛</m:t>
-                            </m:r>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>=6</m:t>
-                            </m:r>
-                          </m:sup>
-                          <m:e>
-                            <m:r>
-                              <a:rPr lang="en-CA" sz="1100" b="0" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>𝑅𝐸𝑉𝐼𝑆𝐼𝑂𝑁𝑛</m:t>
-                            </m:r>
-                          </m:e>
-                        </m:nary>
-                      </m:den>
-                    </m:f>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-CA" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A1B7C9-9C63-492E-A370-27B519FA45EC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8514460" y="2733676"/>
-              <a:ext cx="2315465" cy="628650"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝐴𝑣𝑒𝑟𝑎𝑔𝑒)^ </a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>=</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>∑_(𝑛</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>=</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" b="0" i="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:rPr>
-                <a:t>1)^(𝑛=6)▒𝐶𝐹𝑛   )/(∑_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-CA" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑛=1)^(𝑛=6)▒𝑅𝐸𝑉𝐼𝑆𝐼𝑂𝑁𝑛)</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-CA" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -807,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,13 +569,25 @@
       <c r="B7">
         <v>2798</v>
       </c>
-      <c r="E7" t="e">
+      <c r="C7">
+        <v>165</v>
+      </c>
+      <c r="D7">
+        <v>65</v>
+      </c>
+      <c r="E7">
         <f>C7/D7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H7" t="e">
+        <v>2.5384615384615383</v>
+      </c>
+      <c r="F7">
+        <v>316</v>
+      </c>
+      <c r="G7">
+        <v>65</v>
+      </c>
+      <c r="H7">
         <f>F7/G7</f>
-        <v>#DIV/0!</v>
+        <v>4.8615384615384611</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -978,27 +596,27 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>146</v>
+        <v>311</v>
       </c>
       <c r="D8">
         <f>SUM(D3:D7)</f>
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="E8">
         <f>C8/D8</f>
-        <v>2.2461538461538462</v>
+        <v>2.3923076923076922</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>321</v>
+        <v>637</v>
       </c>
       <c r="G8">
         <f>SUM(G3:G7)</f>
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="H8">
         <f>F8/G8</f>
-        <v>4.9384615384615387</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1037,7 +655,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1398,10 +1015,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45DAA6C-6044-4BDB-98CB-11DB5B63E69A}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,16 +1182,6 @@
         <v>25.454545454545453</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D15" t="e">
-        <f>AVERAGE(D3:D7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G15" t="e">
-        <f>AVERAGE(G3:G7)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>

</xml_diff>

<commit_message>
Implemented for reduced number of revisions.
</commit_message>
<xml_diff>
--- a/Results of ConQat.xlsx
+++ b/Results of ConQat.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7EAF14-62CA-4AE4-A815-72C2946F48E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B995A-3A64-4633-8831-9A84F126C224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="3225" windowWidth="12525" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8160" yWindow="3900" windowWidth="14280" windowHeight="7965" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RQ1" sheetId="1" r:id="rId1"/>
     <sheet name="RQ2" sheetId="2" r:id="rId2"/>
     <sheet name="RQ3" sheetId="3" r:id="rId3"/>
     <sheet name="RQ4" sheetId="4" r:id="rId4"/>
+    <sheet name="RQ5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="20">
   <si>
     <t>Ctags</t>
   </si>
@@ -82,6 +83,15 @@
   </si>
   <si>
     <t>Rep CFs</t>
+  </si>
+  <si>
+    <t>Rep CFs LOCs</t>
+  </si>
+  <si>
+    <t>CFs LOCs</t>
+  </si>
+  <si>
+    <t>For 1545 revisions</t>
   </si>
 </sst>
 </file>
@@ -413,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +436,7 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
     <col min="14" max="14" width="14.28515625" customWidth="1"/>
@@ -537,13 +547,25 @@
       <c r="B5">
         <v>10354</v>
       </c>
-      <c r="E5" t="e">
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
         <f>C5/D5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H5" t="e">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="F5">
+        <v>18</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
         <f>F5/G5</f>
-        <v>#DIV/0!</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -553,13 +575,25 @@
       <c r="B6">
         <v>2886</v>
       </c>
-      <c r="E6" t="e">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
         <f>C6/D6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H6" t="e">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
         <f>F6/G6</f>
-        <v>#DIV/0!</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -570,24 +604,24 @@
         <v>2798</v>
       </c>
       <c r="C7">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <f>C7/D7</f>
-        <v>2.5384615384615383</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>316</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <f>F7/G7</f>
-        <v>4.8615384615384611</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -596,27 +630,58 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>311</v>
+        <v>160</v>
       </c>
       <c r="D8">
         <f>SUM(D3:D7)</f>
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="E8">
         <f>C8/D8</f>
-        <v>2.3923076923076922</v>
+        <v>2.2222222222222223</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>637</v>
+        <v>353</v>
       </c>
       <c r="G8">
         <f>SUM(G3:G7)</f>
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="H8">
         <f>F8/G8</f>
-        <v>4.9000000000000004</v>
+        <v>4.9027777777777777</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2798</v>
+      </c>
+      <c r="C12">
+        <v>117</v>
+      </c>
+      <c r="D12">
+        <v>65</v>
+      </c>
+      <c r="E12">
+        <f>C12/D12</f>
+        <v>1.8</v>
+      </c>
+      <c r="F12">
+        <v>316</v>
+      </c>
+      <c r="G12">
+        <v>65</v>
+      </c>
+      <c r="H12">
+        <f>F12/G12</f>
+        <v>4.8615384615384611</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -663,7 +728,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,39 +826,75 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="e">
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
         <f>B5/C5*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>548</v>
+      </c>
+      <c r="G5">
         <f>E5/F5*100</f>
-        <v>#DIV/0!</v>
+        <v>3.2846715328467155</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6" t="e">
         <f>B6/C6*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G6" t="e">
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
         <f>E6/F6*100</f>
-        <v>#DIV/0!</v>
+        <v>88.888888888888886</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
       <c r="D7" t="e">
         <f>B7/C7*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G7" t="e">
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>147</v>
+      </c>
+      <c r="G7">
         <f>E7/F7*100</f>
-        <v>#DIV/0!</v>
+        <v>4.0816326530612246</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -802,27 +903,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="D8">
         <f>B8/C8*100</f>
-        <v>95.424836601307192</v>
+        <v>95.808383233532936</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>13312</v>
+        <v>14016</v>
       </c>
       <c r="G8">
         <f>E8/F8*100</f>
-        <v>2.4113581730769234</v>
+        <v>2.5185502283105023</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +941,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,39 +1040,75 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="e">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <f>B5/C5*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <f>E5/F5*100</f>
-        <v>#DIV/0!</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="e">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <f>B6/C6*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" t="e">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
         <f>E6/F6*100</f>
-        <v>#DIV/0!</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <f>B7/C7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <f>E7/F7*100</f>
-        <v>#DIV/0!</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,11 +1117,11 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D8">
         <f>B8/C8*100</f>
@@ -992,15 +1129,15 @@
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G8">
         <f>E8/F8*100</f>
-        <v>78.571428571428569</v>
+        <v>77.5</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1155,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,39 +1255,75 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="e">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <f>C5/B5*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" t="e">
+        <v>33.333333333333329</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <f>F5/E5*100</f>
-        <v>#DIV/0!</v>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="e">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <f>C6/B6*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" t="e">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <f>F6/E6*100</f>
-        <v>#DIV/0!</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="e">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <f>C7/B7*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" t="e">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <f>F7/E7*100</f>
-        <v>#DIV/0!</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1159,27 +1332,27 @@
       </c>
       <c r="B8">
         <f>SUM(B3:B7)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <f>C8/B8*100</f>
-        <v>32.142857142857146</v>
+        <v>36.363636363636367</v>
       </c>
       <c r="E8">
         <f>SUM(E3:E7)</f>
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <f>SUM(F3:F7)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G8">
         <f>F8/E8*100</f>
-        <v>25.454545454545453</v>
+        <v>27.419354838709676</v>
       </c>
     </row>
   </sheetData>
@@ -1190,4 +1363,216 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F627D1E7-516A-445E-97B6-DE103BB8B53F}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>437894</v>
+      </c>
+      <c r="C3">
+        <v>5177512</v>
+      </c>
+      <c r="D3">
+        <f>B3/C3*100</f>
+        <v>8.4576143908502761</v>
+      </c>
+      <c r="E3">
+        <v>2925129</v>
+      </c>
+      <c r="F3">
+        <v>17036371</v>
+      </c>
+      <c r="G3">
+        <f>E3/F3*100</f>
+        <v>17.169906666155605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1363688</v>
+      </c>
+      <c r="C4">
+        <v>12733290</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4" si="0">B4/C4*100</f>
+        <v>10.709628069414896</v>
+      </c>
+      <c r="E4">
+        <v>2317473</v>
+      </c>
+      <c r="F4">
+        <v>19098646</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4" si="1">E4/F4*100</f>
+        <v>12.134226688111816</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>202006</v>
+      </c>
+      <c r="C5">
+        <v>3030064</v>
+      </c>
+      <c r="D5">
+        <f>B5/C5*100</f>
+        <v>6.6667238711789594</v>
+      </c>
+      <c r="E5">
+        <v>563836</v>
+      </c>
+      <c r="F5">
+        <v>6576597</v>
+      </c>
+      <c r="G5">
+        <f>E5/F5*100</f>
+        <v>8.5733700879041237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>17116</v>
+      </c>
+      <c r="D6">
+        <f>B6/C6*100</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>9148</v>
+      </c>
+      <c r="F6">
+        <v>47747</v>
+      </c>
+      <c r="G6">
+        <f>E6/F6*100</f>
+        <v>19.15931891008859</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>480701</v>
+      </c>
+      <c r="D7">
+        <f>B7/C7*100</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>46320</v>
+      </c>
+      <c r="F7">
+        <v>705773</v>
+      </c>
+      <c r="G7">
+        <f>E7/F7*100</f>
+        <v>6.5630167206736436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B3:B7)</f>
+        <v>2003588</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C3:C7)</f>
+        <v>21438683</v>
+      </c>
+      <c r="D8">
+        <f>B8/C8*100</f>
+        <v>9.3456673621229438</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E7)</f>
+        <v>5861906</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F3:F7)</f>
+        <v>43465134</v>
+      </c>
+      <c r="G8">
+        <f>E8/F8*100</f>
+        <v>13.486455603702959</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>